<commit_message>
ocultando filas y columnas, inmovilizando paneles
</commit_message>
<xml_diff>
--- a/28. 1BONUS de Excel – Modo Presentación Visual de Informes.xlsx.xlsx
+++ b/28. 1BONUS de Excel – Modo Presentación Visual de Informes.xlsx.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel Maraby\Video Cursos\Excel 2017\Producción\Excel y Word\BONOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAUL\Downloads\Materiales-Para-Descargar\Curso_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A2BA25-9188-466C-B3F5-6A680773B8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{387765B8-A6D8-4B9F-8E14-1C810584CD88}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{387765B8-A6D8-4B9F-8E14-1C810584CD88}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico Parque" sheetId="2" r:id="rId1"/>
     <sheet name="Presupuesto1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -337,7 +347,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -406,7 +416,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -536,7 +546,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -665,7 +675,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -795,7 +805,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -913,7 +923,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-PE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -944,7 +954,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1176023231"/>
@@ -1034,7 +1044,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="es-PE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1065,7 +1075,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1186073007"/>
@@ -1106,7 +1116,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1139,7 +1149,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1185,7 +1195,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1302,7 +1312,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1414,7 +1424,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1444,7 +1454,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2607,7 +2617,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B83643D2-9DAD-428A-880B-94DEF44A9F9E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2618,7 +2628,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8666807" cy="6290272"/>
+    <xdr:ext cx="9293311" cy="6071115"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -3233,20 +3243,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACFC325-6757-4813-94EE-2E9E69B2BEB2}">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="33.4" x14ac:dyDescent="1">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3269,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3288,7 +3298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -3319,7 +3329,7 @@
         <v>3.8595846351773572E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -3350,7 +3360,7 @@
         <v>0.2729277706303988</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -3381,7 +3391,7 @@
         <v>0.23708877044660909</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -3412,7 +3422,7 @@
         <v>1.2130123139128837E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -3443,7 +3453,7 @@
         <v>0.14335600073515897</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -3474,7 +3484,7 @@
         <v>6.8921154199595658E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -3505,7 +3515,7 @@
         <v>5.5136923359676529E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -3536,7 +3546,7 @@
         <v>8.9138026098143724E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -3567,7 +3577,7 @@
         <v>8.27053850395148E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
@@ -3601,7 +3611,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3610,7 +3620,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3619,7 +3629,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3628,7 +3638,7 @@
         <v>1933.3333333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>